<commit_message>
images, word docs, data spreadsheets
images -> added new jpgs corresponding to archaeological sites; data -> added image url paths to field values for archaeological sites. word -> added more description edits to word files.
</commit_message>
<xml_diff>
--- a/data/cats.xlsx
+++ b/data/cats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\Projects\Cats\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\Projects\cats-in-culture\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A3C28F-74F7-4210-BEAA-24ADF24E5108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F9721A-0373-4698-98D3-87260B403637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{1ECB13C9-0744-4957-8AC1-010376719F57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1ECB13C9-0744-4957-8AC1-010376719F57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F91DC8-2191-4FC2-BF68-39B2BAEDFB74}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
data, html, word doc updtaes
Added geojsons of slideshow point locations (cat_slides) and archaeological site points (cat_sites); added bootstrap CDN connection to index.html, minor word doc edits, spreadsheets have been updated with lat lon locations in decimal degrees.
</commit_message>
<xml_diff>
--- a/data/cats.xlsx
+++ b/data/cats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\Projects\cats-in-culture\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F9721A-0373-4698-98D3-87260B403637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533EAC0D-55C0-4465-B04D-B44635F4A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1ECB13C9-0744-4957-8AC1-010376719F57}"/>
+    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{1ECB13C9-0744-4957-8AC1-010376719F57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
     <t>Zoom</t>
   </si>
   <si>
-    <t>CenterLat</t>
-  </si>
-  <si>
-    <t>CenterLong</t>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
   </si>
 </sst>
 </file>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F91DC8-2191-4FC2-BF68-39B2BAEDFB74}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>